<commit_message>
10 Test Cases added
</commit_message>
<xml_diff>
--- a/Players/Bharath/Test Case_Radiology_Bharath.xlsx
+++ b/Players/Bharath/Test Case_Radiology_Bharath.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mediware_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mediware_work\CentralRepository\Players\Bharath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1749F9A9-0E79-4DD0-9A9E-161C2EC4C9B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC94B6D4-AFB0-4E17-8280-538DAEAF07DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="120">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -330,6 +330,113 @@
   </si>
   <si>
     <t>The appoinment should be saved and a green tick mark should be dispayed on the slot</t>
+  </si>
+  <si>
+    <t>Patient ID : NH00000532
+Patient Name : Arun
+Mobile : 67854
+DOB : 28/05/1994</t>
+  </si>
+  <si>
+    <t>Enter data for required field:
+&gt;Patient Id
+or
+&gt;Patient Name
+&gt;Mobile 
+&gt;DOB
+In the Search section</t>
+  </si>
+  <si>
+    <t>Click Search option</t>
+  </si>
+  <si>
+    <t>User should be able to enter the details</t>
+  </si>
+  <si>
+    <t>The patient and details should be displayed</t>
+  </si>
+  <si>
+    <t>Select the patient</t>
+  </si>
+  <si>
+    <t>User should be navigated to the New appoinmnet section with all the details filled out</t>
+  </si>
+  <si>
+    <t>Enter the details for all empty fields</t>
+  </si>
+  <si>
+    <t>User should be able to enter the details for all the empty fields</t>
+  </si>
+  <si>
+    <t>The Appointment should be saved</t>
+  </si>
+  <si>
+    <t>MED_RAD_TC_008</t>
+  </si>
+  <si>
+    <t>Precondition: Patient should be registered
+Login to the URL</t>
+  </si>
+  <si>
+    <t>Test case to verify Show Appoinment  Information</t>
+  </si>
+  <si>
+    <t>Navigate to the central pane &gt;&gt; hover on the required slot where the appoinment is saved &gt;&gt;Click on show appoinment information</t>
+  </si>
+  <si>
+    <t>Details of the patient and the appointment should be displayed</t>
+  </si>
+  <si>
+    <t>MED_RAD_TC_009</t>
+  </si>
+  <si>
+    <t>Navigate to the central pane &gt;&gt; hover on the required slot where the appoinment is saved &gt;&gt;Click on Edit Appointment</t>
+  </si>
+  <si>
+    <t>Precondition: Appointment  should be saved
+Login to the URL</t>
+  </si>
+  <si>
+    <t>Edit Appointment pop-up should be displayed</t>
+  </si>
+  <si>
+    <t>Navigate to the required fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter details or  edit the enabled fields </t>
+  </si>
+  <si>
+    <t>Click on Save option</t>
+  </si>
+  <si>
+    <t>MED_RAD_TC_010</t>
+  </si>
+  <si>
+    <t>Test Case to verify whether a User can Edit an Appointment</t>
+  </si>
+  <si>
+    <t>Test Case to verify whether  a User can cancel an appointment</t>
+  </si>
+  <si>
+    <t>Homepage should be displayed</t>
+  </si>
+  <si>
+    <t>Navigate to the central pane &gt;&gt; hover on the required slot where the appoinment is saved &gt;&gt;Click on Cancel Appointment</t>
+  </si>
+  <si>
+    <t>Cancel Appointment pop-up should be displayed</t>
+  </si>
+  <si>
+    <t>Enter a valid reason in the "Reason of Cancellation" section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter details in the "Reason of Cancellation" section </t>
+  </si>
+  <si>
+    <t>Click on Cancel Appointment option</t>
+  </si>
+  <si>
+    <t>The appointment should be cancelled</t>
   </si>
 </sst>
 </file>
@@ -447,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -536,6 +643,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -875,8 +983,8 @@
   <dimension ref="A1:R737"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +995,7 @@
     <col min="4" max="4" width="23.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="7" customWidth="1"/>
     <col min="6" max="6" width="48.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" style="8" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" style="8" customWidth="1"/>
     <col min="9" max="9" width="15" style="7" customWidth="1"/>
     <col min="10" max="13" width="9.140625" style="7"/>
@@ -932,17 +1040,17 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="Q1" s="32" t="s">
+      <c r="O1" s="32"/>
+      <c r="Q1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="32"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:18" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -951,7 +1059,7 @@
       <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="36" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="7">
@@ -960,10 +1068,12 @@
       <c r="F2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8"/>
       <c r="I2" s="9"/>
       <c r="J2" s="6"/>
       <c r="K2" s="10"/>
@@ -973,7 +1083,7 @@
       </c>
       <c r="O2" s="13">
         <f>COUNTA(A:A)-1</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>15</v>
@@ -984,10 +1094,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="20"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="36"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="27">
         <v>2</v>
       </c>
@@ -1010,10 +1120,10 @@
       <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="20"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="27">
         <v>3</v>
       </c>
@@ -1044,10 +1154,10 @@
       </c>
     </row>
     <row r="5" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="20"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="27">
         <v>4</v>
       </c>
@@ -1075,9 +1185,9 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="20"/>
-      <c r="D6" s="36"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="27">
         <v>5</v>
       </c>
@@ -1098,9 +1208,9 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="20"/>
-      <c r="D7" s="36"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="27">
         <v>6</v>
       </c>
@@ -1117,9 +1227,9 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="20"/>
-      <c r="D8" s="36"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="27">
         <v>7</v>
       </c>
@@ -1133,9 +1243,9 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="20"/>
-      <c r="D9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="27">
         <v>8</v>
       </c>
@@ -1152,9 +1262,9 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="20"/>
-      <c r="D10" s="36"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="27">
         <v>9</v>
       </c>
@@ -1178,11 +1288,11 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="31" t="s">
         <v>40</v>
       </c>
       <c r="E13" s="7">
@@ -1191,17 +1301,20 @@
       <c r="F13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:18" s="23" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="21"/>
       <c r="C14" s="25"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="27">
         <v>2</v>
       </c>
@@ -1218,9 +1331,9 @@
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="5"/>
-      <c r="D15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="27">
         <v>3</v>
       </c>
@@ -1234,9 +1347,9 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="5"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="27">
         <v>4</v>
       </c>
@@ -1250,9 +1363,9 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="5"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="27">
         <v>5</v>
       </c>
@@ -1266,9 +1379,9 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="5"/>
-      <c r="D18" s="30"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="27">
         <v>6</v>
       </c>
@@ -1285,9 +1398,9 @@
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="5"/>
-      <c r="D19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="27">
         <v>7</v>
       </c>
@@ -1306,11 +1419,11 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="31" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="31" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="7">
@@ -1319,17 +1432,19 @@
       <c r="F21" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="28"/>
       <c r="J21" s="6"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="5"/>
-      <c r="D22" s="30"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="27">
         <v>2</v>
       </c>
@@ -1346,9 +1461,9 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="5"/>
-      <c r="D23" s="30"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="27">
         <v>3</v>
       </c>
@@ -1363,9 +1478,9 @@
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="5"/>
-      <c r="D24" s="30"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="27">
         <v>4</v>
       </c>
@@ -1380,9 +1495,9 @@
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="5"/>
-      <c r="D25" s="30"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="27">
         <v>5</v>
       </c>
@@ -1397,9 +1512,9 @@
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="5"/>
-      <c r="D26" s="30"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="27">
         <v>6</v>
       </c>
@@ -1416,9 +1531,9 @@
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="5"/>
-      <c r="D27" s="30"/>
+      <c r="D27" s="31"/>
       <c r="E27" s="27">
         <v>7</v>
       </c>
@@ -1432,9 +1547,9 @@
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="5"/>
-      <c r="D28" s="30"/>
+      <c r="D28" s="31"/>
       <c r="E28" s="27">
         <v>8</v>
       </c>
@@ -1448,9 +1563,9 @@
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="5"/>
-      <c r="D29" s="30"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="27">
         <v>9</v>
       </c>
@@ -1467,9 +1582,9 @@
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="5"/>
-      <c r="D30" s="30"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="27">
         <v>10</v>
       </c>
@@ -1488,11 +1603,11 @@
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="31" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="31" t="s">
         <v>69</v>
       </c>
       <c r="E32" s="7">
@@ -1501,17 +1616,19 @@
       <c r="F32" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H32" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H32" s="28"/>
       <c r="J32" s="6"/>
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="5"/>
-      <c r="D33" s="30"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="27">
         <v>2</v>
       </c>
@@ -1528,9 +1645,9 @@
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="5"/>
-      <c r="D34" s="30"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="27">
         <v>3</v>
       </c>
@@ -1545,9 +1662,9 @@
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="5"/>
-      <c r="D35" s="30"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="27">
         <v>4</v>
       </c>
@@ -1562,9 +1679,9 @@
       <c r="K35" s="10"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5"/>
-      <c r="D36" s="30"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="27">
         <v>5</v>
       </c>
@@ -1579,9 +1696,9 @@
       <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5"/>
-      <c r="D37" s="30"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="27">
         <v>6</v>
       </c>
@@ -1598,9 +1715,9 @@
       <c r="K37" s="10"/>
     </row>
     <row r="38" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5"/>
-      <c r="D38" s="30"/>
+      <c r="D38" s="31"/>
       <c r="E38" s="27">
         <v>7</v>
       </c>
@@ -1615,9 +1732,9 @@
       <c r="K38" s="10"/>
     </row>
     <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5"/>
-      <c r="D39" s="30"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="27">
         <v>8</v>
       </c>
@@ -1632,9 +1749,9 @@
       <c r="K39" s="10"/>
     </row>
     <row r="40" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5"/>
-      <c r="D40" s="30"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="27">
         <v>9</v>
       </c>
@@ -1650,10 +1767,10 @@
       <c r="J40" s="6"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="5"/>
-      <c r="D41" s="30"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="27">
         <v>10</v>
       </c>
@@ -1666,10 +1783,10 @@
       <c r="J41" s="6"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="5"/>
-      <c r="D42" s="30"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="27">
         <v>11</v>
       </c>
@@ -1683,9 +1800,9 @@
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="5"/>
-      <c r="D43" s="30"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="27">
         <v>12</v>
       </c>
@@ -1698,10 +1815,10 @@
       <c r="J43" s="6"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="5"/>
-      <c r="D44" s="30"/>
+      <c r="D44" s="31"/>
       <c r="E44" s="27">
         <v>13</v>
       </c>
@@ -1725,11 +1842,11 @@
       <c r="K46" s="10"/>
     </row>
     <row r="47" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B47" s="5"/>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="31" t="s">
         <v>72</v>
       </c>
       <c r="E47" s="7">
@@ -1738,17 +1855,19 @@
       <c r="F47" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H47" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H47" s="28"/>
       <c r="J47" s="6"/>
       <c r="K47" s="10"/>
     </row>
     <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="5"/>
-      <c r="D48" s="30"/>
+      <c r="D48" s="31"/>
       <c r="E48" s="27">
         <v>2</v>
       </c>
@@ -1765,9 +1884,9 @@
       <c r="K48" s="10"/>
     </row>
     <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="5"/>
-      <c r="D49" s="30"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="27">
         <v>3</v>
       </c>
@@ -1782,9 +1901,9 @@
       <c r="K49" s="10"/>
     </row>
     <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="5"/>
-      <c r="D50" s="30"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="27">
         <v>4</v>
       </c>
@@ -1799,9 +1918,9 @@
       <c r="K50" s="10"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="5"/>
-      <c r="D51" s="30"/>
+      <c r="D51" s="31"/>
       <c r="E51" s="27">
         <v>5</v>
       </c>
@@ -1816,9 +1935,9 @@
       <c r="K51" s="10"/>
     </row>
     <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="5"/>
-      <c r="D52" s="30"/>
+      <c r="D52" s="31"/>
       <c r="E52" s="27">
         <v>6</v>
       </c>
@@ -1835,9 +1954,9 @@
       <c r="K52" s="10"/>
     </row>
     <row r="53" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="5"/>
-      <c r="D53" s="30"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="27">
         <v>7</v>
       </c>
@@ -1852,9 +1971,9 @@
       <c r="K53" s="10"/>
     </row>
     <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
+      <c r="A54" s="31"/>
       <c r="B54" s="5"/>
-      <c r="D54" s="30"/>
+      <c r="D54" s="31"/>
       <c r="E54" s="27">
         <v>8</v>
       </c>
@@ -1869,9 +1988,9 @@
       <c r="K54" s="10"/>
     </row>
     <row r="55" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="31"/>
       <c r="B55" s="5"/>
-      <c r="D55" s="30"/>
+      <c r="D55" s="31"/>
       <c r="E55" s="27">
         <v>9</v>
       </c>
@@ -1887,11 +2006,11 @@
       <c r="J55" s="6"/>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
+    <row r="56" spans="1:11" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
       <c r="B56" s="22"/>
       <c r="C56" s="25"/>
-      <c r="D56" s="30"/>
+      <c r="D56" s="31"/>
       <c r="E56" s="27">
         <v>10</v>
       </c>
@@ -1906,10 +2025,10 @@
       <c r="K56" s="10"/>
     </row>
     <row r="57" spans="1:11" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="22"/>
       <c r="C57" s="25"/>
-      <c r="D57" s="30"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="27">
         <v>11</v>
       </c>
@@ -1926,10 +2045,10 @@
       <c r="K57" s="10"/>
     </row>
     <row r="58" spans="1:11" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="22"/>
       <c r="C58" s="25"/>
-      <c r="D58" s="30"/>
+      <c r="D58" s="31"/>
       <c r="E58" s="27">
         <v>12</v>
       </c>
@@ -1943,10 +2062,10 @@
       <c r="J58" s="25"/>
       <c r="K58" s="10"/>
     </row>
-    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
       <c r="B59" s="5"/>
-      <c r="D59" s="30"/>
+      <c r="D59" s="31"/>
       <c r="E59" s="27">
         <v>13</v>
       </c>
@@ -1960,10 +2079,10 @@
       <c r="J59" s="6"/>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="31"/>
       <c r="B60" s="5"/>
-      <c r="D60" s="30"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="27">
         <v>14</v>
       </c>
@@ -1978,9 +2097,9 @@
       <c r="K60" s="10"/>
     </row>
     <row r="61" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="31"/>
       <c r="B61" s="5"/>
-      <c r="D61" s="30"/>
+      <c r="D61" s="31"/>
       <c r="E61" s="27">
         <v>15</v>
       </c>
@@ -1994,10 +2113,10 @@
       <c r="J61" s="6"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="5"/>
-      <c r="D62" s="30"/>
+      <c r="D62" s="31"/>
       <c r="E62" s="27">
         <v>16</v>
       </c>
@@ -2022,11 +2141,11 @@
       <c r="K64" s="10"/>
     </row>
     <row r="65" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="31" t="s">
         <v>81</v>
       </c>
       <c r="B65" s="5"/>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="31" t="s">
         <v>82</v>
       </c>
       <c r="E65" s="7">
@@ -2035,17 +2154,19 @@
       <c r="F65" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H65" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H65" s="28"/>
       <c r="J65" s="6"/>
       <c r="K65" s="10"/>
     </row>
     <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="5"/>
-      <c r="D66" s="30"/>
+      <c r="D66" s="31"/>
       <c r="E66" s="27">
         <v>2</v>
       </c>
@@ -2062,9 +2183,9 @@
       <c r="K66" s="10"/>
     </row>
     <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="5"/>
-      <c r="D67" s="30"/>
+      <c r="D67" s="31"/>
       <c r="E67" s="27">
         <v>3</v>
       </c>
@@ -2079,9 +2200,9 @@
       <c r="K67" s="10"/>
     </row>
     <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="5"/>
-      <c r="D68" s="30"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="27">
         <v>4</v>
       </c>
@@ -2096,9 +2217,9 @@
       <c r="K68" s="10"/>
     </row>
     <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="5"/>
-      <c r="D69" s="30"/>
+      <c r="D69" s="31"/>
       <c r="E69" s="27">
         <v>5</v>
       </c>
@@ -2113,9 +2234,9 @@
       <c r="K69" s="10"/>
     </row>
     <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="5"/>
-      <c r="D70" s="30"/>
+      <c r="D70" s="31"/>
       <c r="E70" s="27">
         <v>6</v>
       </c>
@@ -2132,9 +2253,9 @@
       <c r="K70" s="10"/>
     </row>
     <row r="71" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="5"/>
-      <c r="D71" s="30"/>
+      <c r="D71" s="31"/>
       <c r="E71" s="27">
         <v>7</v>
       </c>
@@ -2149,9 +2270,9 @@
       <c r="K71" s="10"/>
     </row>
     <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="5"/>
-      <c r="D72" s="30"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="27">
         <v>8</v>
       </c>
@@ -2166,9 +2287,9 @@
       <c r="K72" s="10"/>
     </row>
     <row r="73" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="5"/>
-      <c r="D73" s="30"/>
+      <c r="D73" s="31"/>
       <c r="E73" s="27">
         <v>9</v>
       </c>
@@ -2184,10 +2305,10 @@
       <c r="J73" s="6"/>
       <c r="K73" s="10"/>
     </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
       <c r="B74" s="5"/>
-      <c r="D74" s="30"/>
+      <c r="D74" s="31"/>
       <c r="E74" s="27">
         <v>10</v>
       </c>
@@ -2202,9 +2323,9 @@
       <c r="K74" s="10"/>
     </row>
     <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
+      <c r="A75" s="31"/>
       <c r="B75" s="5"/>
-      <c r="D75" s="30"/>
+      <c r="D75" s="31"/>
       <c r="E75" s="27">
         <v>11</v>
       </c>
@@ -2221,9 +2342,9 @@
       <c r="K75" s="10"/>
     </row>
     <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="31"/>
       <c r="B76" s="5"/>
-      <c r="D76" s="30"/>
+      <c r="D76" s="31"/>
       <c r="E76" s="27">
         <v>12</v>
       </c>
@@ -2238,9 +2359,9 @@
       <c r="K76" s="10"/>
     </row>
     <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="5"/>
-      <c r="D77" s="30"/>
+      <c r="D77" s="31"/>
       <c r="E77" s="27">
         <v>13</v>
       </c>
@@ -2263,26 +2384,36 @@
       <c r="J79" s="6"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+    <row r="80" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B80" s="5"/>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="31" t="s">
         <v>85</v>
       </c>
+      <c r="E80" s="7">
+        <v>1</v>
+      </c>
       <c r="F80" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G80" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G80" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H80" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H80" s="28"/>
       <c r="J80" s="6"/>
       <c r="K80" s="10"/>
     </row>
-    <row r="81" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="31"/>
       <c r="B81" s="5"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="27">
+        <v>2</v>
+      </c>
       <c r="F81" s="28" t="s">
         <v>44</v>
       </c>
@@ -2295,8 +2426,13 @@
       <c r="J81" s="6"/>
       <c r="K81" s="10"/>
     </row>
-    <row r="82" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="31"/>
       <c r="B82" s="5"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="27">
+        <v>3</v>
+      </c>
       <c r="F82" s="28" t="s">
         <v>26</v>
       </c>
@@ -2307,8 +2443,13 @@
       <c r="J82" s="6"/>
       <c r="K82" s="10"/>
     </row>
-    <row r="83" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
       <c r="B83" s="5"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="27">
+        <v>4</v>
+      </c>
       <c r="F83" s="28" t="s">
         <v>28</v>
       </c>
@@ -2319,8 +2460,13 @@
       <c r="J83" s="6"/>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
       <c r="B84" s="5"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="27">
+        <v>5</v>
+      </c>
       <c r="F84" s="28" t="s">
         <v>65</v>
       </c>
@@ -2331,8 +2477,13 @@
       <c r="J84" s="6"/>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
       <c r="B85" s="5"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="27">
+        <v>6</v>
+      </c>
       <c r="F85" s="28" t="s">
         <v>30</v>
       </c>
@@ -2345,8 +2496,13 @@
       <c r="J85" s="6"/>
       <c r="K85" s="10"/>
     </row>
-    <row r="86" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A86" s="31"/>
       <c r="B86" s="5"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="27">
+        <v>7</v>
+      </c>
       <c r="F86" s="28" t="s">
         <v>51</v>
       </c>
@@ -2357,8 +2513,13 @@
       <c r="J86" s="6"/>
       <c r="K86" s="10"/>
     </row>
-    <row r="87" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="31"/>
       <c r="B87" s="5"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="27">
+        <v>8</v>
+      </c>
       <c r="F87" s="28" t="s">
         <v>63</v>
       </c>
@@ -2369,207 +2530,617 @@
       <c r="J87" s="6"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
       <c r="B88" s="5"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="27">
+        <v>9</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="J88" s="6"/>
       <c r="K88" s="10"/>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
       <c r="B89" s="5"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="27">
+        <v>10</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="J89" s="6"/>
       <c r="K89" s="10"/>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
       <c r="B90" s="5"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="27">
+        <v>11</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="J90" s="6"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
       <c r="B91" s="5"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="27">
+        <v>12</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="J91" s="6"/>
       <c r="K91" s="10"/>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
       <c r="B92" s="5"/>
+      <c r="D92" s="31"/>
+      <c r="E92" s="27">
+        <v>13</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="J92" s="6"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B93" s="5"/>
       <c r="J93" s="6"/>
       <c r="K93" s="10"/>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B94" s="5"/>
       <c r="J94" s="6"/>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="B95" s="5"/>
+      <c r="D95" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E95" s="7">
+        <v>1</v>
+      </c>
+      <c r="F95" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G95" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H95" s="28"/>
       <c r="J95" s="6"/>
       <c r="K95" s="10"/>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="31"/>
       <c r="B96" s="5"/>
+      <c r="D96" s="31"/>
+      <c r="E96" s="27">
+        <v>2</v>
+      </c>
+      <c r="F96" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G96" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H96" s="29" t="s">
+        <v>46</v>
+      </c>
       <c r="J96" s="6"/>
       <c r="K96" s="10"/>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="31"/>
       <c r="B97" s="5"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="27">
+        <v>3</v>
+      </c>
+      <c r="F97" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G97" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H97" s="28"/>
       <c r="J97" s="6"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
       <c r="B98" s="5"/>
+      <c r="D98" s="31"/>
+      <c r="E98" s="27">
+        <v>4</v>
+      </c>
+      <c r="F98" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G98" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="28"/>
       <c r="J98" s="6"/>
       <c r="K98" s="10"/>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="31"/>
       <c r="B99" s="5"/>
+      <c r="D99" s="31"/>
+      <c r="E99" s="27">
+        <v>5</v>
+      </c>
+      <c r="F99" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G99" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H99" s="28"/>
       <c r="J99" s="6"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="31"/>
       <c r="B100" s="5"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="27">
+        <v>6</v>
+      </c>
+      <c r="F100" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G100" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H100" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="J100" s="6"/>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
       <c r="B101" s="5"/>
+      <c r="D101" s="31"/>
+      <c r="E101" s="27">
+        <v>7</v>
+      </c>
+      <c r="F101" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G101" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H101" s="28"/>
       <c r="J101" s="6"/>
       <c r="K101" s="10"/>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
       <c r="B102" s="5"/>
+      <c r="D102" s="31"/>
+      <c r="E102" s="27">
+        <v>8</v>
+      </c>
+      <c r="F102" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="G102" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="H102" s="28"/>
       <c r="J102" s="6"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B103" s="5"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
       <c r="J103" s="6"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B104" s="5"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="28"/>
       <c r="J104" s="6"/>
       <c r="K104" s="10"/>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="31" t="s">
+        <v>103</v>
+      </c>
       <c r="B105" s="5"/>
+      <c r="D105" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E105" s="7">
+        <v>1</v>
+      </c>
+      <c r="F105" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G105" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H105" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="J105" s="6"/>
       <c r="K105" s="10"/>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
       <c r="B106" s="5"/>
+      <c r="D106" s="31"/>
+      <c r="E106" s="27">
+        <v>2</v>
+      </c>
+      <c r="F106" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G106" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H106" s="28"/>
       <c r="J106" s="6"/>
       <c r="K106" s="10"/>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
       <c r="B107" s="5"/>
+      <c r="D107" s="31"/>
+      <c r="E107" s="27">
+        <v>3</v>
+      </c>
+      <c r="F107" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G107" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H107" s="28"/>
       <c r="J107" s="6"/>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
       <c r="B108" s="5"/>
+      <c r="D108" s="31"/>
+      <c r="E108" s="27">
+        <v>4</v>
+      </c>
+      <c r="F108" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G108" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="J108" s="6"/>
       <c r="K108" s="10"/>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="31"/>
       <c r="B109" s="5"/>
+      <c r="D109" s="31"/>
+      <c r="E109" s="27">
+        <v>5</v>
+      </c>
+      <c r="F109" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G109" s="28" t="s">
+        <v>66</v>
+      </c>
       <c r="J109" s="6"/>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="31"/>
       <c r="B110" s="5"/>
+      <c r="D110" s="31"/>
+      <c r="E110" s="27">
+        <v>6</v>
+      </c>
+      <c r="F110" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G110" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="J110" s="6"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="31"/>
       <c r="B111" s="5"/>
+      <c r="D111" s="31"/>
+      <c r="E111" s="27">
+        <v>7</v>
+      </c>
+      <c r="F111" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G111" s="28" t="s">
+        <v>47</v>
+      </c>
       <c r="J111" s="6"/>
       <c r="K111" s="10"/>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="31"/>
       <c r="B112" s="5"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="27">
+        <v>8</v>
+      </c>
+      <c r="F112" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="G112" s="28" t="s">
+        <v>106</v>
+      </c>
       <c r="J112" s="6"/>
       <c r="K112" s="10"/>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
       <c r="B113" s="5"/>
+      <c r="D113" s="31"/>
+      <c r="E113" s="27">
+        <v>9</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G113" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="J113" s="6"/>
       <c r="K113" s="10"/>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="31"/>
       <c r="B114" s="5"/>
+      <c r="D114" s="31"/>
+      <c r="E114" s="27">
+        <v>10</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G114" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="J114" s="6"/>
       <c r="K114" s="10"/>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B115" s="5"/>
       <c r="J115" s="6"/>
       <c r="K115" s="10"/>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B116" s="5"/>
       <c r="J116" s="6"/>
       <c r="K116" s="10"/>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="31" t="s">
+        <v>110</v>
+      </c>
       <c r="B117" s="5"/>
+      <c r="D117" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E117" s="7">
+        <v>1</v>
+      </c>
+      <c r="F117" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G117" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H117" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="J117" s="6"/>
       <c r="K117" s="10"/>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
       <c r="B118" s="5"/>
+      <c r="D118" s="31"/>
+      <c r="E118" s="27">
+        <v>2</v>
+      </c>
+      <c r="F118" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G118" s="28" t="s">
+        <v>45</v>
+      </c>
       <c r="J118" s="6"/>
       <c r="K118" s="10"/>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
       <c r="B119" s="5"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="27">
+        <v>3</v>
+      </c>
+      <c r="F119" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G119" s="28" t="s">
+        <v>27</v>
+      </c>
       <c r="J119" s="6"/>
       <c r="K119" s="10"/>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="31"/>
       <c r="B120" s="5"/>
+      <c r="D120" s="31"/>
+      <c r="E120" s="27">
+        <v>4</v>
+      </c>
+      <c r="F120" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G120" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="J120" s="6"/>
       <c r="K120" s="10"/>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="31"/>
       <c r="B121" s="5"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="27">
+        <v>5</v>
+      </c>
+      <c r="F121" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G121" s="28" t="s">
+        <v>66</v>
+      </c>
       <c r="J121" s="6"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
       <c r="B122" s="5"/>
+      <c r="D122" s="31"/>
+      <c r="E122" s="27">
+        <v>6</v>
+      </c>
+      <c r="F122" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G122" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H122" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="J122" s="6"/>
       <c r="K122" s="10"/>
     </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
       <c r="B123" s="5"/>
+      <c r="D123" s="31"/>
+      <c r="E123" s="27">
+        <v>7</v>
+      </c>
+      <c r="F123" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G123" s="28" t="s">
+        <v>47</v>
+      </c>
       <c r="J123" s="6"/>
       <c r="K123" s="10"/>
     </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
       <c r="B124" s="5"/>
+      <c r="D124" s="31"/>
+      <c r="E124" s="27">
+        <v>8</v>
+      </c>
+      <c r="F124" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="G124" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="J124" s="6"/>
       <c r="K124" s="10"/>
     </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
       <c r="B125" s="5"/>
+      <c r="D125" s="31"/>
+      <c r="E125" s="27">
+        <v>9</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G125" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="J125" s="6"/>
       <c r="K125" s="10"/>
     </row>
-    <row r="126" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
       <c r="B126" s="5"/>
+      <c r="D126" s="31"/>
+      <c r="E126" s="27">
+        <v>10</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G126" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="J126" s="6"/>
       <c r="K126" s="10"/>
     </row>
-    <row r="127" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B127" s="5"/>
       <c r="J127" s="6"/>
       <c r="K127" s="10"/>
     </row>
-    <row r="128" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B128" s="5"/>
       <c r="J128" s="6"/>
       <c r="K128" s="10"/>
@@ -5451,13 +6022,9 @@
       <c r="K737" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="D13:D19"/>
+  <mergeCells count="22">
+    <mergeCell ref="A80:A92"/>
+    <mergeCell ref="D80:D92"/>
     <mergeCell ref="A65:A77"/>
     <mergeCell ref="D65:D77"/>
     <mergeCell ref="A21:A30"/>
@@ -5466,6 +6033,18 @@
     <mergeCell ref="D32:D44"/>
     <mergeCell ref="A47:A62"/>
     <mergeCell ref="D47:D62"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="D13:D19"/>
+    <mergeCell ref="A95:A102"/>
+    <mergeCell ref="D95:D102"/>
+    <mergeCell ref="A105:A114"/>
+    <mergeCell ref="D105:D114"/>
+    <mergeCell ref="A117:A126"/>
+    <mergeCell ref="D117:D126"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J489 C2:C663" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5485,15 +6064,17 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G21" r:id="rId3" xr:uid="{6D4A4FFD-9853-4DA8-AD52-5E02B9156723}"/>
-    <hyperlink ref="G32" r:id="rId4" xr:uid="{08C0551B-BED1-4D3B-BB70-34FDD08921D5}"/>
-    <hyperlink ref="G47" r:id="rId5" xr:uid="{ACE0F7C8-FDBB-4B4B-A246-F72E2C249114}"/>
-    <hyperlink ref="G65" r:id="rId6" xr:uid="{3C794EFA-0941-4387-BEDE-1963E2C72278}"/>
-    <hyperlink ref="G80" r:id="rId7" xr:uid="{06A50111-FAB4-4F72-BDE6-C13813D71717}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{DBF75F0E-5DCA-41D6-99F5-6C55E8F08E56}"/>
+    <hyperlink ref="H13" r:id="rId2" xr:uid="{7AAAE32D-CE6C-4687-832F-115484069002}"/>
+    <hyperlink ref="H21" r:id="rId3" xr:uid="{27CDBA63-04DB-4C7B-B4AC-C63351D43E9C}"/>
+    <hyperlink ref="H32" r:id="rId4" xr:uid="{0C18ADEB-F501-458A-BB5E-571DE21ED983}"/>
+    <hyperlink ref="H47" r:id="rId5" xr:uid="{2D90E039-283A-4437-AB07-53BF3E1BCC3F}"/>
+    <hyperlink ref="H65" r:id="rId6" xr:uid="{CB74AC1E-AE33-4A59-95E0-E1805609E9DB}"/>
+    <hyperlink ref="H80" r:id="rId7" xr:uid="{D3E21784-2D5F-4619-8048-9B643B5C9BB0}"/>
+    <hyperlink ref="H117" r:id="rId8" xr:uid="{3A9E708C-D44D-47FD-AF93-A0A997CEE3A1}"/>
+    <hyperlink ref="H105" r:id="rId9" xr:uid="{5163BC5E-5C9C-45C1-B446-0E00EDA155F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>